<commit_message>
duplicate column was finded
</commit_message>
<xml_diff>
--- a/src/assets/excel/sample.xlsx
+++ b/src/assets/excel/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THIRU\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REACH-ON-EXPRESS\frontend\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D9FE73D-D8CC-42CA-A7FC-9C472B34DA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126E836C-5571-4779-8334-35196D899EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{24FCB01B-F29D-42EE-9EE8-5CE86CD1D604}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>leafId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>vendorLeaf</t>
   </si>
@@ -50,22 +47,10 @@
     <t>purchasedDate</t>
   </si>
   <si>
-    <t>RNA100000225</t>
-  </si>
-  <si>
     <t>NM6O9L558998</t>
   </si>
   <si>
     <t>DTDC</t>
-  </si>
-  <si>
-    <t>RNA100010225</t>
-  </si>
-  <si>
-    <t>RNA100020225</t>
-  </si>
-  <si>
-    <t>RNA100030225</t>
   </si>
   <si>
     <t>NM6O9L558999</t>
@@ -453,21 +438,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15669C6-6603-43BB-AF24-2BB13DB90131}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,63 +461,48 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45691</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" s="1">
+        <v>45691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
         <v>45691</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45691</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45691</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
         <v>45691</v>
       </c>
     </row>

</xml_diff>